<commit_message>
Lab03 - WhiteBox definire teste
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28723"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7B8E4903-D725-4331-B45D-1EAD83750DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{072B1A47-CCE9-4DBD-BC0F-A6802FBA147C}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{7B8E4903-D725-4331-B45D-1EAD83750DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F340DFD3-0A0A-48B4-A81F-CB3DEEBE1783}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14856" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14856" firstSheet="3" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="126">
   <si>
     <t>VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -138,33 +138,33 @@
     <t>Source code</t>
   </si>
   <si>
-    <t>Se va insera CFG asociat codului sursa testat (poza, diagrama, etc.).</t>
-  </si>
-  <si>
     <t>CC1 = No. of regions =</t>
   </si>
   <si>
     <t>Req02_L01</t>
   </si>
   <si>
-    <t>31,32</t>
+    <t>35,36</t>
   </si>
   <si>
     <t>CC2 = Edges - Nodes + 2 =</t>
   </si>
   <si>
+    <t>14 - 11 + 2 = 5</t>
+  </si>
+  <si>
     <t>Req02_L02</t>
   </si>
   <si>
-    <t>&lt;Req02 CFG &gt;</t>
-  </si>
-  <si>
     <t>CC3 = No. of Conditions + 1 =</t>
   </si>
   <si>
     <t>Predicate+1</t>
   </si>
   <si>
+    <t>4 + 1= 5</t>
+  </si>
+  <si>
     <t>Req02_L03</t>
   </si>
   <si>
@@ -195,7 +195,7 @@
     <t>F02_P01</t>
   </si>
   <si>
-    <t>1 - 2(F) -4(F)-8-9</t>
+    <t>1 - 2(T) - 3 - 11</t>
   </si>
   <si>
     <t>Req02_L09</t>
@@ -204,19 +204,31 @@
     <t>F02_P02</t>
   </si>
   <si>
-    <t>1 - 2(T) -3-9</t>
+    <t>1 - 2(F) - 4(T) - 5 - 11</t>
+  </si>
+  <si>
+    <t>Req02_L10</t>
   </si>
   <si>
     <t>F02_P03</t>
   </si>
   <si>
-    <t>1-2(F)-4(T)-5(F)-7-4(F)-8-9</t>
+    <t>1 - 2(F) - 4(F) - 6(F) - 10 - 11</t>
+  </si>
+  <si>
+    <t>Req02_L11</t>
   </si>
   <si>
     <t>F02_P04</t>
   </si>
   <si>
-    <t>1 - 2(F) - 4(T) - 5(T) - 6 - 7 - 4(F) - 8 - 9</t>
+    <t>1 - 2(F) - 4(F) - 6(T) - 7(F) - 9 - 6(F) - 10 - 11</t>
+  </si>
+  <si>
+    <t>F02_P05</t>
+  </si>
+  <si>
+    <t>1 - 2(F) - 4(F) - 6(T) - 7(T) - 8 - 9 - 6(F) - 10 - 11</t>
   </si>
   <si>
     <t>F02. totalul incasarilor pentru fiecare tip (CASH/CARD)</t>
@@ -289,7 +301,7 @@
 payment type = CASH</t>
   </si>
   <si>
-    <t>1,2,3,9</t>
+    <t>1, 2, 3, 11</t>
   </si>
   <si>
     <t>x</t>
@@ -302,6 +314,9 @@
 payment type = CASH</t>
   </si>
   <si>
+    <t>1, 2, 4, 5, 11</t>
+  </si>
+  <si>
     <t>F02_TC03</t>
   </si>
   <si>
@@ -309,7 +324,7 @@
 payment type = CASH</t>
   </si>
   <si>
-    <t>1,2,4,5,6,7,8,9</t>
+    <t>1, 2,  4, 6, 7, 8, 9, 6, 10, 11</t>
   </si>
   <si>
     <t>F02_TC04</t>
@@ -331,6 +346,9 @@
   <si>
     <t>payments = [{12.3, CASH}]
 payment type = CARD</t>
+  </si>
+  <si>
+    <t>1, 2,  4, 6, 7, 9, 6, 10, 11</t>
   </si>
   <si>
     <t>WBT Implemented TCs</t>
@@ -828,7 +846,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1014,12 +1032,175 @@
       </left>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
         <color indexed="64"/>
       </right>
       <top/>
@@ -1030,62 +1211,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1094,113 +1223,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
         <color indexed="64"/>
       </right>
       <top/>
@@ -1214,26 +1236,19 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1318,12 +1333,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1333,6 +1349,15 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1345,43 +1370,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1405,7 +1400,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1414,7 +1409,7 @@
     <xf numFmtId="0" fontId="21" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1426,130 +1421,141 @@
     <xf numFmtId="0" fontId="21" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1572,22 +1578,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>350246</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>2656</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>100529</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>10030</xdr:rowOff>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D3189C7-A813-F4EF-140C-8DA228CDAE7C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB35F4F8-65FA-F1C9-7265-D310102A4A86}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7D3189C7-A813-F4EF-140C-8DA228CDAE7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1603,8 +1612,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="350246" y="3462001"/>
-          <a:ext cx="4079522" cy="2192224"/>
+          <a:off x="571500" y="3838575"/>
+          <a:ext cx="3971925" cy="2286000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1615,23 +1624,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>593417</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>168584</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>80920</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>6743</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECED342F-BF64-5292-A1EF-4A6E77910398}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E0DF38B-354C-9DF9-8000-42CBC2E9AB17}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{EB35F4F8-65FA-F1C9-7265-D310102A4A86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1647,8 +1659,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4922656" y="1261009"/>
-          <a:ext cx="4342724" cy="4571999"/>
+          <a:off x="4886325" y="1676400"/>
+          <a:ext cx="4010025" cy="4391025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1963,12 +1975,12 @@
   <sheetData>
     <row r="1" spans="2:16">
       <c r="B1" s="9"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="2:16">
       <c r="B2" s="26" t="s">
@@ -2088,394 +2100,507 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:T24"/>
+  <dimension ref="B1:T36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:K3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20:T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="17" max="17" width="10.7109375" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" customWidth="1"/>
+    <col min="20" max="20" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20">
       <c r="B1" s="9"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="45"/>
     </row>
     <row r="3" spans="2:20">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="48"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="52"/>
     </row>
     <row r="6" spans="2:20">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="Q6" s="42" t="s">
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="Q6" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
     </row>
     <row r="8" spans="2:20">
       <c r="B8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="9"/>
+      <c r="Q8" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="Q8" s="59" t="s">
+      <c r="R8" s="53"/>
+      <c r="S8" s="53"/>
+      <c r="T8" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="15">
+      <c r="B9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="R8" s="59"/>
-      <c r="S8" s="59"/>
-      <c r="T8" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:20">
-      <c r="B9" s="22" t="s">
+      <c r="C9" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="23"/>
       <c r="G9" s="23"/>
       <c r="I9" s="25"/>
-      <c r="Q9" s="59" t="s">
+      <c r="Q9" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="R9" s="53"/>
+      <c r="S9" s="53"/>
+      <c r="T9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="R9" s="59"/>
-      <c r="S9" s="59"/>
-      <c r="T9" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20">
+    </row>
+    <row r="10" spans="2:20" ht="14.45" customHeight="1">
       <c r="B10" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="49">
-        <v>33</v>
-      </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
+      <c r="C10" s="48">
+        <v>37</v>
+      </c>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
-      <c r="I10" s="50" t="s">
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="Q10" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="52"/>
-      <c r="Q10" s="59" t="s">
+      <c r="R10" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="R10" s="59" t="s">
+      <c r="S10" s="53"/>
+      <c r="T10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="S10" s="59"/>
-      <c r="T10" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20">
+    </row>
+    <row r="11" spans="2:20" ht="14.45" customHeight="1">
       <c r="B11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="49">
-        <v>34</v>
-      </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
+      <c r="C11" s="48">
+        <v>38</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="54"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="55"/>
-    </row>
-    <row r="12" spans="2:20">
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+    </row>
+    <row r="12" spans="2:20" ht="14.45" customHeight="1">
       <c r="B12" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="49">
-        <v>35</v>
-      </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
+      <c r="C12" s="48">
+        <v>39</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="55"/>
-    </row>
-    <row r="13" spans="2:20">
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+    </row>
+    <row r="13" spans="2:20" ht="14.45" customHeight="1">
       <c r="B13" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="49">
-        <v>36</v>
-      </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
+      <c r="C13" s="48">
+        <v>40</v>
+      </c>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="55"/>
-      <c r="Q13" s="42" t="s">
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="Q13" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="R13" s="43"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="43"/>
-    </row>
-    <row r="14" spans="2:20">
+      <c r="R13" s="44"/>
+      <c r="S13" s="44"/>
+      <c r="T13" s="44"/>
+    </row>
+    <row r="14" spans="2:20" ht="14.45" customHeight="1">
       <c r="B14" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="61">
-        <v>37</v>
-      </c>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
+      <c r="C14" s="55">
+        <v>31</v>
+      </c>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="55"/>
-    </row>
-    <row r="15" spans="2:20">
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+    </row>
+    <row r="15" spans="2:20" ht="14.45" customHeight="1">
       <c r="B15" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="49">
-        <v>38</v>
-      </c>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="55"/>
+      <c r="C15" s="48">
+        <v>42</v>
+      </c>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
       <c r="Q15" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="R15" s="60" t="s">
+      <c r="R15" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60"/>
-    </row>
-    <row r="16" spans="2:20">
+      <c r="S15" s="54"/>
+      <c r="T15" s="54"/>
+    </row>
+    <row r="16" spans="2:20" ht="14.45" customHeight="1">
       <c r="B16" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="61">
-        <v>39</v>
-      </c>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="55"/>
+      <c r="C16" s="55">
+        <v>43</v>
+      </c>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
       <c r="Q16" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="R16" s="45" t="s">
+      <c r="R16" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-    </row>
-    <row r="17" spans="2:20">
+      <c r="S16" s="49"/>
+      <c r="T16" s="49"/>
+    </row>
+    <row r="17" spans="2:20" ht="14.45" customHeight="1">
       <c r="B17" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="49">
-        <v>40</v>
-      </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="55"/>
+      <c r="C17" s="48">
+        <v>44</v>
+      </c>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
       <c r="Q17" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="R17" s="45" t="s">
+      <c r="R17" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
-    </row>
-    <row r="18" spans="2:20">
-      <c r="B18" s="28"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="55"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+    </row>
+    <row r="18" spans="2:20" ht="14.45" customHeight="1">
+      <c r="B18" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="48">
+        <v>45</v>
+      </c>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="47"/>
       <c r="Q18" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="R18" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-    </row>
-    <row r="19" spans="2:20">
-      <c r="I19" s="53"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="55"/>
+      <c r="R18" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+    </row>
+    <row r="19" spans="2:20" ht="14.45" customHeight="1">
+      <c r="B19" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="48">
+        <v>46</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
       <c r="Q19" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="R19" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="S19" s="45"/>
-      <c r="T19" s="45"/>
-    </row>
-    <row r="20" spans="2:20">
-      <c r="I20" s="53"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="55"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="45"/>
-      <c r="S20" s="45"/>
-      <c r="T20" s="45"/>
-    </row>
-    <row r="21" spans="2:20">
-      <c r="I21" s="53"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="55"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="45"/>
-      <c r="S21" s="45"/>
-      <c r="T21" s="45"/>
-    </row>
-    <row r="22" spans="2:20">
-      <c r="I22" s="53"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="55"/>
-    </row>
-    <row r="23" spans="2:20">
-      <c r="I23" s="53"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="55"/>
-    </row>
-    <row r="24" spans="2:20">
-      <c r="I24" s="56"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="57"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="58"/>
-    </row>
+        <v>49</v>
+      </c>
+      <c r="R19" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+    </row>
+    <row r="20" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
+      <c r="Q20" s="113" t="s">
+        <v>51</v>
+      </c>
+      <c r="R20" s="114" t="s">
+        <v>52</v>
+      </c>
+      <c r="S20" s="114"/>
+      <c r="T20" s="114"/>
+    </row>
+    <row r="21" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="Q21" s="111"/>
+      <c r="R21" s="112"/>
+      <c r="S21" s="112"/>
+      <c r="T21" s="112"/>
+    </row>
+    <row r="22" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="47"/>
+    </row>
+    <row r="23" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="47"/>
+    </row>
+    <row r="24" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="47"/>
+    </row>
+    <row r="25" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="47"/>
+    </row>
+    <row r="26" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+    </row>
+    <row r="27" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="47"/>
+    </row>
+    <row r="28" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="47"/>
+    </row>
+    <row r="29" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
+    </row>
+    <row r="30" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="47"/>
+    </row>
+    <row r="31" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="47"/>
+      <c r="O31" s="47"/>
+    </row>
+    <row r="32" spans="2:20" ht="14.45" customHeight="1">
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="47"/>
+    </row>
+    <row r="33" spans="9:15" ht="14.45" customHeight="1">
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="47"/>
+      <c r="O33" s="47"/>
+    </row>
+    <row r="34" spans="9:15" ht="14.45" customHeight="1">
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="47"/>
+    </row>
+    <row r="35" spans="9:15" ht="14.45" customHeight="1">
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+    </row>
+    <row r="36" spans="9:15" ht="15"/>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
+    <mergeCell ref="R19:T19"/>
     <mergeCell ref="R18:T18"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="Q9:S9"/>
@@ -2488,12 +2613,13 @@
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C18:E18"/>
+    <mergeCell ref="I10:O35"/>
+    <mergeCell ref="C19:E19"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="R21:T21"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="C10:E10"/>
-    <mergeCell ref="I10:O24"/>
     <mergeCell ref="Q10:S10"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="R15:T15"/>
@@ -2503,7 +2629,6 @@
     <mergeCell ref="I6:O6"/>
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R19:T19"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2517,13 +2642,13 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:X16"/>
+  <dimension ref="B1:Y16"/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="A6" zoomScale="89" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="32"/>
     <col min="2" max="2" width="12.28515625" style="32" customWidth="1"/>
@@ -2540,504 +2665,517 @@
     <col min="13" max="13" width="23.85546875" style="32" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="32" customWidth="1"/>
     <col min="15" max="15" width="8.85546875" style="32" customWidth="1"/>
-    <col min="16" max="17" width="8.85546875" style="32"/>
-    <col min="18" max="18" width="2.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="2.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5" style="32" customWidth="1"/>
-    <col min="22" max="22" width="2.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6" style="32" customWidth="1"/>
-    <col min="24" max="24" width="5.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.85546875" style="32"/>
+    <col min="16" max="18" width="8.85546875" style="32"/>
+    <col min="19" max="19" width="2.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="2.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5" style="32" customWidth="1"/>
+    <col min="23" max="23" width="2.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6" style="32" customWidth="1"/>
+    <col min="25" max="25" width="5.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.85546875" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24">
+    <row r="1" spans="2:25">
       <c r="B1" s="31"/>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64"/>
-    </row>
-    <row r="3" spans="2:24">
-      <c r="B3" s="65" t="s">
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="58"/>
+    </row>
+    <row r="3" spans="2:25">
+      <c r="B3" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="61"/>
+    </row>
+    <row r="5" spans="2:25">
+      <c r="B5" s="33"/>
+    </row>
+    <row r="6" spans="2:25" ht="15.75">
+      <c r="B6" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="62"/>
+      <c r="W6" s="62"/>
+      <c r="X6" s="62"/>
+      <c r="Y6" s="62"/>
+    </row>
+    <row r="7" spans="2:25" ht="15.75">
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="69"/>
+      <c r="P7" s="69"/>
+      <c r="Q7" s="69"/>
+      <c r="R7" s="69"/>
+      <c r="S7" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="T7" s="65"/>
+      <c r="U7" s="65"/>
+      <c r="V7" s="65"/>
+      <c r="W7" s="65"/>
+      <c r="X7" s="65"/>
+      <c r="Y7" s="65"/>
+    </row>
+    <row r="8" spans="2:25" ht="15.6" customHeight="1">
+      <c r="B8" s="62"/>
+      <c r="C8" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="70"/>
+      <c r="F8" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" s="68"/>
+      <c r="L8" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="M8" s="72"/>
+      <c r="N8" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="O8" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="P8" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="67"/>
-    </row>
-    <row r="5" spans="2:24">
-      <c r="B5" s="33"/>
-    </row>
-    <row r="6" spans="2:24" ht="15.6">
-      <c r="B6" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="68" t="s">
+      <c r="R8" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="69" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="68" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="68"/>
-      <c r="Q6" s="68"/>
-      <c r="R6" s="68"/>
-      <c r="S6" s="68"/>
-      <c r="T6" s="68"/>
-      <c r="U6" s="68"/>
-      <c r="V6" s="68"/>
-      <c r="W6" s="68"/>
-      <c r="X6" s="68"/>
-    </row>
-    <row r="7" spans="2:24" ht="15.6">
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="78" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="74" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="75" t="s">
-        <v>56</v>
-      </c>
-      <c r="O7" s="75"/>
-      <c r="P7" s="75"/>
-      <c r="Q7" s="75"/>
-      <c r="R7" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="S7" s="71"/>
-      <c r="T7" s="71"/>
-      <c r="U7" s="71"/>
-      <c r="V7" s="71"/>
-      <c r="W7" s="71"/>
-      <c r="X7" s="71"/>
-    </row>
-    <row r="8" spans="2:24" ht="15.6" customHeight="1">
-      <c r="B8" s="68"/>
-      <c r="C8" s="72" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="72" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="78"/>
-      <c r="F8" s="74" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74" t="s">
-        <v>62</v>
-      </c>
-      <c r="K8" s="74"/>
-      <c r="L8" s="76" t="s">
-        <v>63</v>
-      </c>
-      <c r="M8" s="77"/>
-      <c r="N8" s="75" t="s">
-        <v>40</v>
-      </c>
-      <c r="O8" s="75" t="s">
-        <v>43</v>
-      </c>
-      <c r="P8" s="75" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q8" s="75" t="s">
-        <v>47</v>
-      </c>
-      <c r="R8" s="71">
+      <c r="S8" s="65">
         <v>0</v>
       </c>
-      <c r="S8" s="71">
+      <c r="T8" s="65">
         <v>1</v>
       </c>
-      <c r="T8" s="71">
+      <c r="U8" s="65">
         <v>2</v>
       </c>
-      <c r="U8" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="V8" s="71" t="s">
-        <v>65</v>
-      </c>
-      <c r="W8" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="X8" s="71" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="2:24" ht="15.6">
-      <c r="B9" s="68"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="78"/>
+      <c r="V8" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="W8" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="X8" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y8" s="65" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" ht="16.5">
+      <c r="B9" s="62"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="70"/>
       <c r="F9" s="34" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="I9" s="34" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="K9" s="34" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="M9" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="N9" s="75"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="75"/>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="71"/>
-      <c r="S9" s="71"/>
-      <c r="T9" s="71"/>
-      <c r="U9" s="71"/>
-      <c r="V9" s="71"/>
-      <c r="W9" s="71"/>
-      <c r="X9" s="71"/>
-    </row>
-    <row r="10" spans="2:24" ht="31.15">
+        <v>73</v>
+      </c>
+      <c r="N9" s="69"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="69"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="65"/>
+      <c r="T9" s="65"/>
+      <c r="U9" s="65"/>
+      <c r="V9" s="65"/>
+      <c r="W9" s="65"/>
+      <c r="X9" s="65"/>
+      <c r="Y9" s="65"/>
+    </row>
+    <row r="10" spans="2:25" ht="32.25">
       <c r="B10" s="29" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D10" s="30">
         <v>0</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G10" s="36"/>
       <c r="H10" s="36"/>
       <c r="I10" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="L10" s="36"/>
       <c r="M10" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37" t="s">
-        <v>73</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="N10" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="O10" s="37"/>
       <c r="P10" s="37"/>
       <c r="Q10" s="37"/>
-      <c r="R10" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="S10" s="38"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="38" t="s">
+        <v>77</v>
+      </c>
       <c r="T10" s="38"/>
       <c r="U10" s="38"/>
       <c r="V10" s="38"/>
       <c r="W10" s="38"/>
       <c r="X10" s="38"/>
-    </row>
-    <row r="11" spans="2:24" ht="31.15">
+      <c r="Y10" s="38"/>
+    </row>
+    <row r="11" spans="2:25" ht="32.25">
       <c r="B11" s="29" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D11" s="30">
         <v>0</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F11" s="36"/>
       <c r="G11" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H11" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="L11" s="36"/>
       <c r="M11" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="N11" s="37"/>
       <c r="O11" s="37" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="P11" s="37"/>
       <c r="Q11" s="37"/>
-      <c r="R11" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="S11" s="38"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="38" t="s">
+        <v>77</v>
+      </c>
       <c r="T11" s="38"/>
       <c r="U11" s="38"/>
       <c r="V11" s="38"/>
       <c r="W11" s="38"/>
       <c r="X11" s="38"/>
-    </row>
-    <row r="12" spans="2:24" ht="31.15">
+      <c r="Y11" s="38"/>
+    </row>
+    <row r="12" spans="2:25" ht="32.25">
       <c r="B12" s="29" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D12" s="30">
         <v>12.3</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K12" s="36"/>
       <c r="L12" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M12" s="36"/>
       <c r="N12" s="37"/>
       <c r="O12" s="37"/>
       <c r="P12" s="37"/>
-      <c r="Q12" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="R12" s="38"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37" t="s">
+        <v>77</v>
+      </c>
       <c r="S12" s="38"/>
       <c r="T12" s="38"/>
       <c r="U12" s="38"/>
-      <c r="V12" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="W12" s="38"/>
+      <c r="V12" s="38"/>
+      <c r="W12" s="38" t="s">
+        <v>77</v>
+      </c>
       <c r="X12" s="38"/>
-    </row>
-    <row r="13" spans="2:24" ht="31.15">
+      <c r="Y12" s="38"/>
+    </row>
+    <row r="13" spans="2:25" ht="32.25">
       <c r="B13" s="29" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D13" s="30">
         <v>0</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
       <c r="I13" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="J13" s="36"/>
       <c r="K13" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="L13" s="36"/>
       <c r="M13" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37" t="s">
-        <v>73</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="N13" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="O13" s="37"/>
       <c r="P13" s="37"/>
       <c r="Q13" s="37"/>
-      <c r="R13" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="S13" s="38"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="38" t="s">
+        <v>77</v>
+      </c>
       <c r="T13" s="38"/>
       <c r="U13" s="38"/>
       <c r="V13" s="38"/>
       <c r="W13" s="38"/>
       <c r="X13" s="38"/>
-    </row>
-    <row r="14" spans="2:24" ht="31.15">
+      <c r="Y13" s="38"/>
+    </row>
+    <row r="14" spans="2:25" ht="32.25">
       <c r="B14" s="29" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D14" s="30">
         <v>0</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F14" s="36"/>
       <c r="G14" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H14" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="I14" s="36"/>
       <c r="J14" s="36"/>
       <c r="K14" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="L14" s="36"/>
       <c r="M14" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="N14" s="37"/>
       <c r="O14" s="37" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="P14" s="37"/>
       <c r="Q14" s="37"/>
-      <c r="R14" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="S14" s="38"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="38" t="s">
+        <v>77</v>
+      </c>
       <c r="T14" s="38"/>
       <c r="U14" s="38"/>
       <c r="V14" s="38"/>
       <c r="W14" s="38"/>
       <c r="X14" s="38"/>
-    </row>
-    <row r="15" spans="2:24" ht="31.15">
+      <c r="Y14" s="38"/>
+    </row>
+    <row r="15" spans="2:25" ht="32.25">
       <c r="B15" s="29" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D15" s="30">
         <v>0</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="F15" s="36"/>
       <c r="G15" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H15" s="36"/>
       <c r="I15" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K15" s="36"/>
       <c r="L15" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M15" s="36"/>
       <c r="N15" s="37"/>
       <c r="O15" s="37"/>
-      <c r="P15" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="38"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="R15" s="37"/>
       <c r="S15" s="38"/>
       <c r="T15" s="38"/>
       <c r="U15" s="38"/>
-      <c r="V15" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="W15" s="38"/>
+      <c r="V15" s="38"/>
+      <c r="W15" s="38" t="s">
+        <v>77</v>
+      </c>
       <c r="X15" s="38"/>
-    </row>
-    <row r="16" spans="2:24" ht="15.6">
+      <c r="Y15" s="38"/>
+    </row>
+    <row r="16" spans="2:25" ht="15.75">
       <c r="B16" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="28">
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:M7"/>
-    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="N7:R7"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="S8:S9"/>
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="R8:R9"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:X6"/>
-    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="E6:Y6"/>
     <mergeCell ref="W8:W9"/>
+    <mergeCell ref="X8:X9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="S8:S9"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="U8:U9"/>
-    <mergeCell ref="R7:X7"/>
-    <mergeCell ref="X8:X9"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="S7:Y7"/>
+    <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="H8:I8"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
@@ -3053,8 +3191,8 @@
   </sheetPr>
   <dimension ref="B1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -3074,104 +3212,104 @@
   <sheetData>
     <row r="1" spans="2:14">
       <c r="B1" s="9"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="3" spans="2:14">
-      <c r="B3" s="81" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
+      <c r="B3" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
     </row>
     <row r="4" spans="2:14">
-      <c r="B4" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="92" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="94" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="84" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="84" t="s">
-        <v>90</v>
-      </c>
-      <c r="L4" s="85"/>
+      <c r="B4" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="88" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="78" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="78" t="s">
+        <v>96</v>
+      </c>
+      <c r="L4" s="79"/>
     </row>
     <row r="5" spans="2:14">
-      <c r="B5" s="83"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="95"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="89"/>
       <c r="E5" s="40" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="I5" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="J5" s="87"/>
+        <v>99</v>
+      </c>
+      <c r="I5" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="81"/>
       <c r="K5" s="40" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="L5" s="40" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="2:14">
       <c r="B6" s="27">
         <v>9</v>
       </c>
-      <c r="C6" s="88" t="s">
-        <v>96</v>
+      <c r="C6" s="82" t="s">
+        <v>102</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G6" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" s="84" t="s">
-        <v>93</v>
-      </c>
-      <c r="J6" s="85"/>
+      <c r="I6" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="79"/>
       <c r="K6" s="10">
         <v>0</v>
       </c>
@@ -3183,26 +3321,26 @@
       <c r="B7" s="27">
         <v>10</v>
       </c>
-      <c r="C7" s="89"/>
+      <c r="C7" s="83"/>
       <c r="D7" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="G7" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="I7" s="84" t="s">
-        <v>93</v>
-      </c>
-      <c r="J7" s="85"/>
+      <c r="I7" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="J7" s="79"/>
       <c r="K7" s="10">
         <v>0</v>
       </c>
@@ -3214,26 +3352,26 @@
       <c r="B8" s="27">
         <v>11</v>
       </c>
-      <c r="C8" s="89"/>
+      <c r="C8" s="83"/>
       <c r="D8" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="G8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="I8" s="84" t="s">
-        <v>93</v>
-      </c>
-      <c r="J8" s="85"/>
+      <c r="I8" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="79"/>
       <c r="K8" s="10">
         <v>12.3</v>
       </c>
@@ -3245,26 +3383,26 @@
       <c r="B9" s="27">
         <v>12</v>
       </c>
-      <c r="C9" s="89"/>
+      <c r="C9" s="83"/>
       <c r="D9" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G9" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="I9" s="84" t="s">
-        <v>93</v>
-      </c>
-      <c r="J9" s="85"/>
+      <c r="I9" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" s="79"/>
       <c r="K9" s="10">
         <v>0</v>
       </c>
@@ -3276,26 +3414,26 @@
       <c r="B10" s="27">
         <v>13</v>
       </c>
-      <c r="C10" s="90"/>
+      <c r="C10" s="84"/>
       <c r="D10" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="G10" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="I10" s="84" t="s">
-        <v>93</v>
-      </c>
-      <c r="J10" s="85"/>
+      <c r="I10" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="J10" s="79"/>
       <c r="K10" s="10">
         <v>0</v>
       </c>
@@ -3309,24 +3447,24 @@
       </c>
       <c r="C11" s="41"/>
       <c r="D11" s="10" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="G11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="I11" s="84" t="s">
-        <v>93</v>
-      </c>
-      <c r="J11" s="85"/>
+      <c r="I11" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="J11" s="79"/>
       <c r="K11" s="10">
         <v>0</v>
       </c>
@@ -3336,88 +3474,88 @@
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1">
       <c r="B12" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="K12" s="11"/>
     </row>
     <row r="13" spans="2:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="B13" s="96" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="98" t="s">
-        <v>105</v>
-      </c>
-      <c r="G13" s="99"/>
-      <c r="H13" s="96" t="s">
-        <v>106</v>
-      </c>
-      <c r="I13" s="97"/>
-      <c r="J13" s="97"/>
-      <c r="K13" s="97"/>
-      <c r="L13" s="113"/>
-      <c r="M13" s="79" t="s">
-        <v>107</v>
-      </c>
-      <c r="N13" s="80"/>
+      <c r="B13" s="90" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="G13" s="93"/>
+      <c r="H13" s="90" t="s">
+        <v>112</v>
+      </c>
+      <c r="I13" s="91"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="91"/>
+      <c r="L13" s="107"/>
+      <c r="M13" s="73" t="s">
+        <v>113</v>
+      </c>
+      <c r="N13" s="74"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickTop="1">
-      <c r="B14" s="108" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="104" t="s">
-        <v>109</v>
-      </c>
-      <c r="D14" s="104" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" s="110" t="s">
-        <v>111</v>
-      </c>
-      <c r="F14" s="101" t="s">
-        <v>112</v>
-      </c>
-      <c r="G14" s="100" t="s">
-        <v>113</v>
-      </c>
-      <c r="H14" s="102" t="s">
+      <c r="B14" s="102" t="s">
         <v>114</v>
       </c>
-      <c r="I14" s="104" t="s">
-        <v>108</v>
-      </c>
-      <c r="J14" s="104" t="s">
-        <v>109</v>
-      </c>
-      <c r="K14" s="106" t="s">
+      <c r="C14" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="L14" s="114" t="s">
+      <c r="D14" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="M14" s="116" t="s">
+      <c r="E14" s="104" t="s">
         <v>117</v>
       </c>
-      <c r="N14" s="92" t="s">
+      <c r="F14" s="95" t="s">
         <v>118</v>
       </c>
+      <c r="G14" s="94" t="s">
+        <v>119</v>
+      </c>
+      <c r="H14" s="96" t="s">
+        <v>120</v>
+      </c>
+      <c r="I14" s="98" t="s">
+        <v>114</v>
+      </c>
+      <c r="J14" s="98" t="s">
+        <v>115</v>
+      </c>
+      <c r="K14" s="100" t="s">
+        <v>121</v>
+      </c>
+      <c r="L14" s="108" t="s">
+        <v>122</v>
+      </c>
+      <c r="M14" s="110" t="s">
+        <v>123</v>
+      </c>
+      <c r="N14" s="86" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="15" spans="2:14" ht="67.900000000000006" customHeight="1">
-      <c r="B15" s="109"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="111"/>
-      <c r="F15" s="112"/>
-      <c r="G15" s="100"/>
-      <c r="H15" s="103"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="107"/>
-      <c r="L15" s="115"/>
-      <c r="M15" s="108"/>
-      <c r="N15" s="101"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="106"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="99"/>
+      <c r="K15" s="101"/>
+      <c r="L15" s="109"/>
+      <c r="M15" s="102"/>
+      <c r="N15" s="95"/>
     </row>
     <row r="16" spans="2:14">
       <c r="B16" s="14">
@@ -3429,17 +3567,17 @@
       <c r="D16" s="12">
         <v>0</v>
       </c>
-      <c r="E16" s="117">
+      <c r="E16" s="42">
         <v>1</v>
       </c>
       <c r="F16" s="13">
         <v>0</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="I16" s="14">
         <f>SUM(J16:K16)</f>
@@ -3453,7 +3591,7 @@
       </c>
       <c r="L16" s="16"/>
       <c r="M16" s="5" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N16" s="17">
         <f>C16</f>
@@ -3502,21 +3640,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d50638930d08c51b5585735b2be047e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4acb07121b76573bb3c966f3dcb1b903" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -3660,14 +3783,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741A764F-DFF5-4AE4-B0E7-77BD148FABB8}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741A764F-DFF5-4AE4-B0E7-77BD148FABB8}"/>
 </file>
</xml_diff>